<commit_message>
FE graph, without sources yet.
</commit_message>
<xml_diff>
--- a/chapters/ch08-Transportation/datasets/Fleet FE Performance.xlsx
+++ b/chapters/ch08-Transportation/datasets/Fleet FE Performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MCBook2021/chapters/ch08-Transportation/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C649706E-4175-D847-8438-12F2AE66BC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F37845-87D4-2247-A368-8DD79AD162F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="43">
   <si>
     <t>CAFE Public Information Center Reports</t>
   </si>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t>www.nhtsa.gov/cafe_pic.html</t>
-  </si>
-  <si>
-    <t>Model Year</t>
   </si>
   <si>
     <t>Light Truck [mpg]</t>
@@ -887,7 +884,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1004,6 +1001,9 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1156,82 +1156,82 @@
               <c:strCache>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>1978</c:v>
+                  <c:v>1978.00</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1979</c:v>
+                  <c:v>1979.00</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1980</c:v>
+                  <c:v>1980.00</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1981</c:v>
+                  <c:v>1981.00</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1982</c:v>
+                  <c:v>1982.00</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1983</c:v>
+                  <c:v>1983.00</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1984</c:v>
+                  <c:v>1984.00</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1985</c:v>
+                  <c:v>1985.00</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1986</c:v>
+                  <c:v>1986.00</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1987</c:v>
+                  <c:v>1987.00</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1988</c:v>
+                  <c:v>1988.00</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1989</c:v>
+                  <c:v>1989.00</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1990</c:v>
+                  <c:v>1990.00</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1991</c:v>
+                  <c:v>1991.00</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1992</c:v>
+                  <c:v>1992.00</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1993</c:v>
+                  <c:v>1993.00</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1994</c:v>
+                  <c:v>1994.00</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1995</c:v>
+                  <c:v>1995.00</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1996</c:v>
+                  <c:v>1996.00</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1997</c:v>
+                  <c:v>1997.00</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1998</c:v>
+                  <c:v>1998.00</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1999</c:v>
+                  <c:v>1999.00</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2000</c:v>
+                  <c:v>2000.00</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2001</c:v>
+                  <c:v>2001.00</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2002</c:v>
+                  <c:v>2002.00</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2003</c:v>
+                  <c:v>2003.00</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>2004</c:v>
@@ -1456,82 +1456,82 @@
               <c:strCache>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>1978</c:v>
+                  <c:v>1978.00</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1979</c:v>
+                  <c:v>1979.00</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1980</c:v>
+                  <c:v>1980.00</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1981</c:v>
+                  <c:v>1981.00</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1982</c:v>
+                  <c:v>1982.00</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1983</c:v>
+                  <c:v>1983.00</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1984</c:v>
+                  <c:v>1984.00</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1985</c:v>
+                  <c:v>1985.00</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1986</c:v>
+                  <c:v>1986.00</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1987</c:v>
+                  <c:v>1987.00</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1988</c:v>
+                  <c:v>1988.00</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1989</c:v>
+                  <c:v>1989.00</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1990</c:v>
+                  <c:v>1990.00</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1991</c:v>
+                  <c:v>1991.00</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1992</c:v>
+                  <c:v>1992.00</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1993</c:v>
+                  <c:v>1993.00</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1994</c:v>
+                  <c:v>1994.00</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1995</c:v>
+                  <c:v>1995.00</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1996</c:v>
+                  <c:v>1996.00</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1997</c:v>
+                  <c:v>1997.00</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1998</c:v>
+                  <c:v>1998.00</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1999</c:v>
+                  <c:v>1999.00</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2000</c:v>
+                  <c:v>2000.00</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2001</c:v>
+                  <c:v>2001.00</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2002</c:v>
+                  <c:v>2002.00</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2003</c:v>
+                  <c:v>2003.00</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>2004</c:v>
@@ -1753,82 +1753,82 @@
               <c:strCache>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>1978</c:v>
+                  <c:v>1978.00</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1979</c:v>
+                  <c:v>1979.00</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1980</c:v>
+                  <c:v>1980.00</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1981</c:v>
+                  <c:v>1981.00</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1982</c:v>
+                  <c:v>1982.00</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1983</c:v>
+                  <c:v>1983.00</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1984</c:v>
+                  <c:v>1984.00</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1985</c:v>
+                  <c:v>1985.00</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1986</c:v>
+                  <c:v>1986.00</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1987</c:v>
+                  <c:v>1987.00</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1988</c:v>
+                  <c:v>1988.00</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1989</c:v>
+                  <c:v>1989.00</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1990</c:v>
+                  <c:v>1990.00</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1991</c:v>
+                  <c:v>1991.00</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1992</c:v>
+                  <c:v>1992.00</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1993</c:v>
+                  <c:v>1993.00</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1994</c:v>
+                  <c:v>1994.00</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1995</c:v>
+                  <c:v>1995.00</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1996</c:v>
+                  <c:v>1996.00</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1997</c:v>
+                  <c:v>1997.00</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1998</c:v>
+                  <c:v>1998.00</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1999</c:v>
+                  <c:v>1999.00</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2000</c:v>
+                  <c:v>2000.00</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2001</c:v>
+                  <c:v>2001.00</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2002</c:v>
+                  <c:v>2002.00</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2003</c:v>
+                  <c:v>2003.00</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>2004</c:v>
@@ -3284,7 +3284,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A41" sqref="A2:A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3297,23 +3297,23 @@
   <sheetData>
     <row r="1" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="37" t="s">
+      <c r="D1" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="36" t="s">
-        <v>30</v>
-      </c>
       <c r="E1" s="38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="36">
+      <c r="A2" s="39">
         <f>'Earlier data'!A2</f>
         <v>1978</v>
       </c>
@@ -3327,11 +3327,11 @@
         <v>19.899999999999999</v>
       </c>
       <c r="E2" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="36">
+      <c r="A3" s="39">
         <f>'Earlier data'!A3</f>
         <v>1979</v>
       </c>
@@ -3348,11 +3348,11 @@
         <v>20.100000000000001</v>
       </c>
       <c r="E3" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="36">
+      <c r="A4" s="39">
         <f>'Earlier data'!A4</f>
         <v>1980</v>
       </c>
@@ -3369,11 +3369,11 @@
         <v>23.1</v>
       </c>
       <c r="E4" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="36">
+      <c r="A5" s="39">
         <f>'Earlier data'!A5</f>
         <v>1981</v>
       </c>
@@ -3390,11 +3390,11 @@
         <v>24.6</v>
       </c>
       <c r="E5" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="36">
+      <c r="A6" s="39">
         <f>'Earlier data'!A6</f>
         <v>1982</v>
       </c>
@@ -3411,11 +3411,11 @@
         <v>25.1</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="36">
+      <c r="A7" s="39">
         <f>'Earlier data'!A7</f>
         <v>1983</v>
       </c>
@@ -3432,11 +3432,11 @@
         <v>24.8</v>
       </c>
       <c r="E7" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="36">
+      <c r="A8" s="39">
         <f>'Earlier data'!A8</f>
         <v>1984</v>
       </c>
@@ -3453,11 +3453,11 @@
         <v>25</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="36">
+      <c r="A9" s="39">
         <f>'Earlier data'!A9</f>
         <v>1985</v>
       </c>
@@ -3474,11 +3474,11 @@
         <v>25.4</v>
       </c>
       <c r="E9" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="36">
+      <c r="A10" s="39">
         <f>'Earlier data'!A10</f>
         <v>1986</v>
       </c>
@@ -3495,11 +3495,11 @@
         <v>25.9</v>
       </c>
       <c r="E10" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="36">
+      <c r="A11" s="39">
         <f>'Earlier data'!A11</f>
         <v>1987</v>
       </c>
@@ -3516,11 +3516,11 @@
         <v>26.2</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="36">
+      <c r="A12" s="39">
         <f>'Earlier data'!A12</f>
         <v>1988</v>
       </c>
@@ -3537,11 +3537,11 @@
         <v>26</v>
       </c>
       <c r="E12" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="36">
+      <c r="A13" s="39">
         <f>'Earlier data'!A13</f>
         <v>1989</v>
       </c>
@@ -3558,11 +3558,11 @@
         <v>25.6</v>
       </c>
       <c r="E13" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="36">
+      <c r="A14" s="39">
         <f>'Earlier data'!A14</f>
         <v>1990</v>
       </c>
@@ -3579,11 +3579,11 @@
         <v>25.4</v>
       </c>
       <c r="E14" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="36">
+      <c r="A15" s="39">
         <f>'Earlier data'!A15</f>
         <v>1991</v>
       </c>
@@ -3600,11 +3600,11 @@
         <v>25.6</v>
       </c>
       <c r="E15" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="36">
+      <c r="A16" s="39">
         <f>'Earlier data'!A16</f>
         <v>1992</v>
       </c>
@@ -3621,11 +3621,11 @@
         <v>25.1</v>
       </c>
       <c r="E16" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="36">
+      <c r="A17" s="39">
         <f>'Earlier data'!A17</f>
         <v>1993</v>
       </c>
@@ -3642,11 +3642,11 @@
         <v>25.2</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="36">
+      <c r="A18" s="39">
         <f>'Earlier data'!A18</f>
         <v>1994</v>
       </c>
@@ -3663,11 +3663,11 @@
         <v>24.7</v>
       </c>
       <c r="E18" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="36">
+      <c r="A19" s="39">
         <f>'Earlier data'!A19</f>
         <v>1995</v>
       </c>
@@ -3684,11 +3684,11 @@
         <v>24.9</v>
       </c>
       <c r="E19" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="36">
+      <c r="A20" s="39">
         <f>'Earlier data'!A20</f>
         <v>1996</v>
       </c>
@@ -3705,11 +3705,11 @@
         <v>24.9</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="36">
+      <c r="A21" s="39">
         <f>'Earlier data'!A21</f>
         <v>1997</v>
       </c>
@@ -3726,11 +3726,11 @@
         <v>24.6</v>
       </c>
       <c r="E21" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="36">
+      <c r="A22" s="39">
         <f>'Earlier data'!A22</f>
         <v>1998</v>
       </c>
@@ -3747,11 +3747,11 @@
         <v>24.7</v>
       </c>
       <c r="E22" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="36">
+      <c r="A23" s="39">
         <f>'Earlier data'!A23</f>
         <v>1999</v>
       </c>
@@ -3768,11 +3768,11 @@
         <v>24.5</v>
       </c>
       <c r="E23" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="36">
+      <c r="A24" s="39">
         <f>'Earlier data'!A24</f>
         <v>2000</v>
       </c>
@@ -3789,11 +3789,11 @@
         <v>24.8</v>
       </c>
       <c r="E24" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="36">
+      <c r="A25" s="39">
         <f>'Earlier data'!A25</f>
         <v>2001</v>
       </c>
@@ -3810,11 +3810,11 @@
         <v>24.5</v>
       </c>
       <c r="E25" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="36">
+      <c r="A26" s="39">
         <f>'Earlier data'!A26</f>
         <v>2002</v>
       </c>
@@ -3831,11 +3831,11 @@
         <v>24.7</v>
       </c>
       <c r="E26" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="38" customFormat="1" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="36">
+      <c r="A27" s="39">
         <f>'Earlier data'!A27</f>
         <v>2003</v>
       </c>
@@ -3852,7 +3852,7 @@
         <v>25.1</v>
       </c>
       <c r="E27" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
@@ -3873,7 +3873,7 @@
         <v>24.6</v>
       </c>
       <c r="E28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
@@ -3894,7 +3894,7 @@
         <v>25.4</v>
       </c>
       <c r="E29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
@@ -3915,7 +3915,7 @@
         <v>25.8</v>
       </c>
       <c r="E30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
@@ -3936,7 +3936,7 @@
         <v>26.6</v>
       </c>
       <c r="E31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
@@ -3957,7 +3957,7 @@
         <v>27.1</v>
       </c>
       <c r="E32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
@@ -3978,7 +3978,7 @@
         <v>29</v>
       </c>
       <c r="E33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
@@ -3999,7 +3999,7 @@
         <v>29.3</v>
       </c>
       <c r="E34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
@@ -4020,7 +4020,7 @@
         <v>29</v>
       </c>
       <c r="E35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
@@ -4041,7 +4041,7 @@
         <v>30.8</v>
       </c>
       <c r="E36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
@@ -4062,7 +4062,7 @@
         <v>31.6</v>
       </c>
       <c r="E37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
@@ -4083,7 +4083,7 @@
         <v>31.7</v>
       </c>
       <c r="E38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
@@ -4104,7 +4104,7 @@
         <v>32.200000000000003</v>
       </c>
       <c r="E39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
@@ -4125,7 +4125,7 @@
         <v>32.299999999999997</v>
       </c>
       <c r="E40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
@@ -4146,7 +4146,7 @@
         <v>33.4</v>
       </c>
       <c r="E41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
@@ -4198,7 +4198,7 @@
       </c>
       <c r="B2" s="26"/>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -4289,7 +4289,7 @@
       <c r="M11" s="31"/>
       <c r="N11" s="24"/>
       <c r="P11" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="3" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -5027,16 +5027,16 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>37</v>
-      </c>
-      <c r="D1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.15">
@@ -5050,7 +5050,7 @@
         <v>19.899999999999999</v>
       </c>
       <c r="W2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.15">
@@ -5067,7 +5067,7 @@
         <v>18.2</v>
       </c>
       <c r="W3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.15">
@@ -5084,7 +5084,7 @@
         <v>18.5</v>
       </c>
       <c r="W4" s="35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.15">

</xml_diff>